<commit_message>
Mapping Daily Weather Report stations to British Rainfall
</commit_message>
<xml_diff>
--- a/DailyReadings/DailyWeatherReports/Comparisons/PORTLAND-BILL2-DWR-1900-1910-Comparison.xlsx
+++ b/DailyReadings/DailyWeatherReports/Comparisons/PORTLAND-BILL2-DWR-1900-1910-Comparison.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Key" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Comparisons!$A$2:$G$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Comparisons!$A$2:$G$35</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2510" uniqueCount="188">
   <si>
     <t>Series 1</t>
   </si>
@@ -503,6 +503,57 @@
     <t>23.39</t>
   </si>
   <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>PORTLAND-BILL-2.csv</t>
+  </si>
+  <si>
+    <t>1.11</t>
+  </si>
+  <si>
+    <t>0.71</t>
+  </si>
+  <si>
+    <t>26.59</t>
+  </si>
+  <si>
+    <t>0.36</t>
+  </si>
+  <si>
+    <t>1.37</t>
+  </si>
+  <si>
+    <t>4.38</t>
+  </si>
+  <si>
+    <t>0.95</t>
+  </si>
+  <si>
+    <t>20.01</t>
+  </si>
+  <si>
+    <t>5.00</t>
+  </si>
+  <si>
+    <t>26.98</t>
+  </si>
+  <si>
+    <t>2.69</t>
+  </si>
+  <si>
+    <t>2.75</t>
+  </si>
+  <si>
+    <t>4.06</t>
+  </si>
+  <si>
+    <t>25.98</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -515,13 +566,7 @@
     <t>Values are the same on both sheets</t>
   </si>
   <si>
-    <t>~</t>
-  </si>
-  <si>
     <t>Values differ by less than 0.1</t>
-  </si>
-  <si>
-    <t>+</t>
   </si>
   <si>
     <t>Values differ by 0.1 or more</t>
@@ -1072,7 +1117,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BG18"/>
+  <dimension ref="A1:BG34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
@@ -1114,7 +1159,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>6</v>
@@ -1196,7 +1241,7 @@
         <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -1249,7 +1294,7 @@
     </row>
     <row r="3" spans="1:59">
       <c r="H3" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:59">
@@ -1275,7 +1320,7 @@
         <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>10</v>
@@ -1445,7 +1490,7 @@
         <v>30</v>
       </c>
       <c r="H5" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -1615,7 +1660,7 @@
         <v>30</v>
       </c>
       <c r="H6" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="I6" s="14" t="s">
         <v>12</v>
@@ -1785,7 +1830,7 @@
         <v>30</v>
       </c>
       <c r="H7" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="I7" s="14" t="s">
         <v>13</v>
@@ -1955,7 +2000,7 @@
         <v>30</v>
       </c>
       <c r="H8" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="I8" s="14" t="s">
         <v>14</v>
@@ -2125,7 +2170,7 @@
         <v>30</v>
       </c>
       <c r="H9" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="I9" s="14" t="s">
         <v>15</v>
@@ -2295,7 +2340,7 @@
         <v>30</v>
       </c>
       <c r="H10" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="I10" s="14" t="s">
         <v>16</v>
@@ -2465,7 +2510,7 @@
         <v>30</v>
       </c>
       <c r="H11" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="I11" s="14" t="s">
         <v>17</v>
@@ -2635,7 +2680,7 @@
         <v>30</v>
       </c>
       <c r="H12" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="I12" s="14" t="s">
         <v>18</v>
@@ -2805,7 +2850,7 @@
         <v>30</v>
       </c>
       <c r="H13" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="I13" s="14" t="s">
         <v>19</v>
@@ -2975,7 +3020,7 @@
         <v>30</v>
       </c>
       <c r="H14" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="I14" s="14" t="s">
         <v>20</v>
@@ -3145,7 +3190,7 @@
         <v>30</v>
       </c>
       <c r="H15" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="I15" s="14" t="s">
         <v>21</v>
@@ -3315,7 +3360,7 @@
         <v>30</v>
       </c>
       <c r="H16" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="I16" s="14" t="s">
         <v>22</v>
@@ -3485,7 +3530,7 @@
         <v>30</v>
       </c>
       <c r="H17" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="I17" s="17" t="s">
         <v>23</v>
@@ -3655,11 +3700,2422 @@
         <v>30</v>
       </c>
       <c r="H18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:59">
+      <c r="H19" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:59">
+      <c r="A20" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" t="s">
+        <v>178</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="10">
+        <v>1900</v>
+      </c>
+      <c r="K20" s="10">
+        <v>1901</v>
+      </c>
+      <c r="L20" s="10">
+        <v>1902</v>
+      </c>
+      <c r="M20" s="10">
+        <v>1903</v>
+      </c>
+      <c r="N20" s="10">
+        <v>1904</v>
+      </c>
+      <c r="O20" s="10">
+        <v>1905</v>
+      </c>
+      <c r="P20" s="10">
+        <v>1906</v>
+      </c>
+      <c r="Q20" s="10">
+        <v>1907</v>
+      </c>
+      <c r="R20" s="10">
+        <v>1908</v>
+      </c>
+      <c r="S20" s="10">
+        <v>1909</v>
+      </c>
+      <c r="T20" s="11">
+        <v>1910</v>
+      </c>
+      <c r="V20" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="W20" s="10">
+        <v>1900</v>
+      </c>
+      <c r="X20" s="10">
+        <v>1901</v>
+      </c>
+      <c r="Y20" s="10">
+        <v>1902</v>
+      </c>
+      <c r="Z20" s="10">
+        <v>1903</v>
+      </c>
+      <c r="AA20" s="10">
+        <v>1904</v>
+      </c>
+      <c r="AB20" s="10">
+        <v>1905</v>
+      </c>
+      <c r="AC20" s="10">
+        <v>1906</v>
+      </c>
+      <c r="AD20" s="10">
+        <v>1907</v>
+      </c>
+      <c r="AE20" s="10">
+        <v>1908</v>
+      </c>
+      <c r="AF20" s="10">
+        <v>1909</v>
+      </c>
+      <c r="AG20" s="11">
+        <v>1910</v>
+      </c>
+      <c r="AI20" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ20" s="10">
+        <v>1900</v>
+      </c>
+      <c r="AK20" s="10">
+        <v>1901</v>
+      </c>
+      <c r="AL20" s="10">
+        <v>1902</v>
+      </c>
+      <c r="AM20" s="10">
+        <v>1903</v>
+      </c>
+      <c r="AN20" s="10">
+        <v>1904</v>
+      </c>
+      <c r="AO20" s="10">
+        <v>1905</v>
+      </c>
+      <c r="AP20" s="10">
+        <v>1906</v>
+      </c>
+      <c r="AQ20" s="10">
+        <v>1907</v>
+      </c>
+      <c r="AR20" s="10">
+        <v>1908</v>
+      </c>
+      <c r="AS20" s="10">
+        <v>1909</v>
+      </c>
+      <c r="AT20" s="11">
+        <v>1910</v>
+      </c>
+      <c r="AV20" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AW20" s="10">
+        <v>1900</v>
+      </c>
+      <c r="AX20" s="10">
+        <v>1901</v>
+      </c>
+      <c r="AY20" s="10">
+        <v>1902</v>
+      </c>
+      <c r="AZ20" s="10">
+        <v>1903</v>
+      </c>
+      <c r="BA20" s="10">
+        <v>1904</v>
+      </c>
+      <c r="BB20" s="10">
+        <v>1905</v>
+      </c>
+      <c r="BC20" s="10">
+        <v>1906</v>
+      </c>
+      <c r="BD20" s="10">
+        <v>1907</v>
+      </c>
+      <c r="BE20" s="10">
+        <v>1908</v>
+      </c>
+      <c r="BF20" s="10">
+        <v>1909</v>
+      </c>
+      <c r="BG20" s="11">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="21" spans="1:59">
+      <c r="A21" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" t="s">
+        <v>178</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="O21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q21" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="R21" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="S21" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="T21" s="16" t="s">
         <v>161</v>
+      </c>
+      <c r="V21" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="W21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="X21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD21" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG21" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="AI21" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AQ21" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR21" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS21" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="AT21" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV21" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AW21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AX21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AZ21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BA21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BC21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BD21" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="BE21" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF21" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG21" s="16" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:59">
+      <c r="A22" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" t="s">
+        <v>178</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="O22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q22" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="R22" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="S22" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="T22" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="V22" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="W22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="X22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD22" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="16">
+        <v>0</v>
+      </c>
+      <c r="AI22" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AQ22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR22" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="AS22" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT22" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="AV22" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AX22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AZ22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BA22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BC22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BD22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="BE22" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="BF22" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="BG22" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:59">
+      <c r="A23" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" t="s">
+        <v>178</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="O23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q23" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="R23" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="S23" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="T23" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="V23" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="W23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="X23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD23" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG23" s="16">
+        <v>0</v>
+      </c>
+      <c r="AI23" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AQ23" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AR23" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS23" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="AT23" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="AV23" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AW23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AX23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AZ23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BA23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BC23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BD23" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="BE23" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="BF23" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="BG23" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:59">
+      <c r="A24" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" t="s">
+        <v>178</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="O24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q24" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="R24" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="S24" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="T24" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="V24" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="W24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="X24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD24" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE24" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG24" s="16">
+        <v>0</v>
+      </c>
+      <c r="AI24" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AQ24" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="AR24" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="AS24" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="AT24" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="AV24" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AW24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AX24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AZ24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BA24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BC24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BD24" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="BE24" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF24" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="BG24" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:59">
+      <c r="A25" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" t="s">
+        <v>178</v>
+      </c>
+      <c r="I25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="O25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P25" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q25" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="R25" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="S25" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="T25" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="V25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="W25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="X25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC25" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD25" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE25" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG25" s="16">
+        <v>0</v>
+      </c>
+      <c r="AI25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP25" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ25" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="AR25" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS25" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT25" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AX25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AZ25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BA25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BC25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BD25" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="BE25" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="BF25" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="BG25" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:59">
+      <c r="A26" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" t="s">
+        <v>178</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="O26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P26" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q26" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="R26" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="S26" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="T26" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="V26" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="W26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="X26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC26" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD26" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG26" s="16">
+        <v>0</v>
+      </c>
+      <c r="AI26" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP26" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ26" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="AR26" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS26" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="AT26" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="AV26" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="AW26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AX26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AZ26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BA26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BC26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BD26" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="BE26" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="BF26" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="BG26" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:59">
+      <c r="A27" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" t="s">
+        <v>178</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="O27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P27" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q27" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="R27" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="S27" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="T27" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="V27" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="W27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="X27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC27" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD27" s="15">
+        <v>-0.08</v>
+      </c>
+      <c r="AE27" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF27" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG27" s="16">
+        <v>0</v>
+      </c>
+      <c r="AI27" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP27" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AQ27" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR27" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS27" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT27" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV27" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="AW27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AX27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AZ27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BA27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BC27" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BD27" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="BE27" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="BF27" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="BG27" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="28" spans="1:59">
+      <c r="A28" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" t="s">
+        <v>178</v>
+      </c>
+      <c r="I28" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="O28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P28" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q28" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="R28" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="S28" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="T28" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="V28" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="W28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="X28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC28" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD28" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="AF28" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG28" s="16">
+        <v>0</v>
+      </c>
+      <c r="AI28" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJ28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP28" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ28" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="AR28" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="AS28" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="AT28" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="AV28" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="AW28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AX28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AZ28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BA28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BC28" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BD28" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="BE28" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="BF28" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="BG28" s="16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:59">
+      <c r="A29" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" t="s">
+        <v>178</v>
+      </c>
+      <c r="I29" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="O29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P29" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q29" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="R29" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="S29" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="T29" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="V29" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="W29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="X29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC29" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD29" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF29" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG29" s="16">
+        <v>0</v>
+      </c>
+      <c r="AI29" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP29" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="AQ29" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR29" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS29" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT29" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="AV29" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="AW29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AX29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AZ29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BA29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BC29" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BD29" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="BE29" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="BF29" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="BG29" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:59">
+      <c r="A30" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" t="s">
+        <v>178</v>
+      </c>
+      <c r="I30" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="O30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P30" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q30" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="R30" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="S30" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="T30" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="V30" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="W30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="X30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC30" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD30" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE30" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="AF30" s="15">
+        <v>-0.12</v>
+      </c>
+      <c r="AG30" s="16">
+        <v>-0.38</v>
+      </c>
+      <c r="AI30" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP30" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AQ30" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR30" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS30" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT30" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="AV30" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="AW30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AX30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AZ30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BA30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BC30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BD30" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="BE30" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="BF30" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="BG30" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="1:59">
+      <c r="A31" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" t="s">
+        <v>178</v>
+      </c>
+      <c r="I31" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="O31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P31" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q31" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="R31" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="S31" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="T31" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="V31" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="W31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="X31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC31" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD31" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="15">
+        <v>0.02</v>
+      </c>
+      <c r="AF31" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG31" s="16">
+        <v>0</v>
+      </c>
+      <c r="AI31" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP31" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ31" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR31" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS31" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT31" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="AV31" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="AW31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AX31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AZ31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BA31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BC31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BD31" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="BE31" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="BF31" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="BG31" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:59">
+      <c r="A32" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H32" t="s">
+        <v>178</v>
+      </c>
+      <c r="I32" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="O32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P32" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q32" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="R32" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="S32" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="T32" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="V32" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="W32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="X32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC32" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD32" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF32" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG32" s="16">
+        <v>0</v>
+      </c>
+      <c r="AI32" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP32" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ32" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR32" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="AS32" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AT32" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="AV32" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="AW32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AX32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AZ32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BA32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BC32" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="BD32" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="BE32" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="BF32" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="BG32" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:59">
+      <c r="A33" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33" t="s">
+        <v>178</v>
+      </c>
+      <c r="I33" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="L33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="N33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="O33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="P33" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q33" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="R33" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="S33" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="T33" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="V33" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="W33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="X33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC33" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD33" s="18">
+        <v>-0.08</v>
+      </c>
+      <c r="AE33" s="18">
+        <v>0.33</v>
+      </c>
+      <c r="AF33" s="18">
+        <v>-0.12</v>
+      </c>
+      <c r="AG33" s="19">
+        <v>-0.36</v>
+      </c>
+      <c r="AI33" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="AJ33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP33" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="AQ33" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR33" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS33" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="AT33" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="AV33" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="AW33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AX33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AY33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AZ33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="BA33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="BC33" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="BD33" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="BE33" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="BF33" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="BG33" s="19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" spans="1:59">
+      <c r="A34" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H34" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G19"/>
+  <autoFilter ref="A2:G35"/>
   <mergeCells count="10">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
@@ -3672,7 +6128,7 @@
     <mergeCell ref="AV1:BG1"/>
     <mergeCell ref="AV2:BG2"/>
   </mergeCells>
-  <conditionalFormatting sqref="AI1:AT19">
+  <conditionalFormatting sqref="AI1:AT35">
     <cfRule type="cellIs" dxfId="3" priority="18" operator="equal">
       <formula>"E"</formula>
     </cfRule>
@@ -3680,7 +6136,7 @@
       <formula>LEFT(AI1,3)="Err"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AV1:BG19">
+  <conditionalFormatting sqref="AV1:BG35">
     <cfRule type="cellIs" dxfId="3" priority="20" operator="equal">
       <formula>"E"</formula>
     </cfRule>
@@ -3688,7 +6144,7 @@
       <formula>LEFT(AV1,3)="Err"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:T19">
+  <conditionalFormatting sqref="I1:T35">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"="</formula>
     </cfRule>
@@ -3711,7 +6167,7 @@
       <formula>"&gt;"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V1:AG19">
+  <conditionalFormatting sqref="V1:AG35">
     <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
       <formula>"E"</formula>
     </cfRule>
@@ -3765,10 +6221,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="7" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3776,23 +6232,23 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3800,7 +6256,7 @@
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3808,7 +6264,7 @@
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -3816,7 +6272,7 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3824,7 +6280,7 @@
         <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>